<commit_message>
Create 7 environment test
</commit_message>
<xml_diff>
--- a/Log Approximate CCP/src/com/robotics/data/Enviroment.xlsx
+++ b/Log Approximate CCP/src/com/robotics/data/Enviroment.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Coverage-Path-Planning\Robotics-Coverage-Path-Planning Version 3\Robotics-Coverage-Path-Planning\Log Approximate CCP\src\com\robotics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C92EA1-7BFA-425E-89B8-E1D56709AC24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9FF382-D0DC-4B8E-9813-935C8FCE2BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E2A9E6F8-C186-4864-91A9-6198DE04BC59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{E2A9E6F8-C186-4864-91A9-6198DE04BC59}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment 1" sheetId="1" r:id="rId1"/>
     <sheet name="Environment 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Environment 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Environment 4" sheetId="5" r:id="rId4"/>
+    <sheet name="Environment 5" sheetId="6" r:id="rId5"/>
+    <sheet name="Environment 6" sheetId="7" r:id="rId6"/>
+    <sheet name="Environment 7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,13 +109,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1930F370-CF85-4540-A7E2-811BBD5A8C2C}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
@@ -883,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197170F0-D02E-496B-8E59-22AAB6C554C4}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,4 +1338,1761 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D636A5A-7B94-43AD-B3C1-D03AC62FF219}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67AC5BE-957E-4938-9581-B60B3E2D14A1}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11:T15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84063E24-8F62-4CC9-98B5-EAEE0B645922}">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D9A750-2606-4E62-8FA9-0014A77FA090}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9221BC1B-AA32-4E38-B1CA-834207B1D235}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>